<commit_message>
add links to project
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L112"/>
+  <dimension ref="A1:L82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -544,12 +544,12 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>۳ روز و  ۱۱ ساعت</t>
+          <t>۳ روز و  ۱۰ ساعت</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615602&amp;domainType=1431&amp;needId=3400618</t>
         </is>
       </c>
     </row>
@@ -602,12 +602,12 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>۴ روز و  ۱۳ ساعت</t>
+          <t>۴ روز و  ۱۲ ساعت</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615556&amp;domainType=1431&amp;needId=3400579</t>
         </is>
       </c>
     </row>
@@ -660,12 +660,12 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>۱ روز و  ۱۹ ساعت</t>
+          <t>۱ روز و  ۱۸ ساعت</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615576&amp;domainType=1431&amp;needId=3400597</t>
         </is>
       </c>
     </row>
@@ -718,12 +718,12 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>۱۳ روز و  ۱۱ ساعت</t>
+          <t>۱۳ روز و  ۱۰ ساعت</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615516&amp;domainType=1431&amp;needId=3400549</t>
         </is>
       </c>
     </row>
@@ -776,12 +776,12 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>۳ روز و  ۱۱ ساعت</t>
+          <t>۳ روز و  ۱۰ ساعت</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615391&amp;domainType=1431&amp;needId=3400437</t>
         </is>
       </c>
     </row>
@@ -834,12 +834,12 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>۴ روز و  ۱۳ ساعت</t>
+          <t>۴ روز و  ۱۲ ساعت</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615499&amp;domainType=1431&amp;needId=3400536</t>
         </is>
       </c>
     </row>
@@ -892,12 +892,12 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>۱ روز و  ۱۹ ساعت</t>
+          <t>۱ روز و  ۱۸ ساعت</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615507&amp;domainType=1431&amp;needId=3400540</t>
         </is>
       </c>
     </row>
@@ -950,12 +950,12 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>۲ روز و  ۱۱ ساعت</t>
+          <t>۲ روز و  ۱۰ ساعت</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615501&amp;domainType=1431&amp;needId=3400533</t>
         </is>
       </c>
     </row>
@@ -1008,12 +1008,12 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>۳ روز و  ۱۵ ساعت</t>
+          <t>۳ روز و  ۱۴ ساعت</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615481&amp;domainType=1431&amp;needId=3400513</t>
         </is>
       </c>
     </row>
@@ -1066,12 +1066,12 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>۲ روز و  ۱۸ ساعت</t>
+          <t>۲ روز و  ۱۷ ساعت</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615444&amp;domainType=1431&amp;needId=3400475</t>
         </is>
       </c>
     </row>
@@ -1124,12 +1124,12 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>۳ روز و  ۱۱ ساعت</t>
+          <t>۳ روز و  ۱۰ ساعت</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615469&amp;domainType=1431&amp;needId=3400500</t>
         </is>
       </c>
     </row>
@@ -1182,12 +1182,12 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>۱۶ روز و  ۸ ساعت</t>
+          <t>۱۶ روز و  ۷ ساعت</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615459&amp;domainType=1431&amp;needId=3400493</t>
         </is>
       </c>
     </row>
@@ -1240,12 +1240,12 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>۳ روز و  ۱۵ ساعت</t>
+          <t>۳ روز و  ۱۴ ساعت</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615453&amp;domainType=1431&amp;needId=3400483</t>
         </is>
       </c>
     </row>
@@ -1298,12 +1298,12 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>۳ روز و  ۱۰ ساعت</t>
+          <t>۳ روز و  ۹ ساعت</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615418&amp;domainType=1431&amp;needId=3400456</t>
         </is>
       </c>
     </row>
@@ -1356,12 +1356,12 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>۳ روز و  ۱۱ ساعت</t>
+          <t>۳ روز و  ۱۰ ساعت</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615436&amp;domainType=1431&amp;needId=3400469</t>
         </is>
       </c>
     </row>
@@ -1414,12 +1414,12 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>۱۴ روز و  ۸ ساعت</t>
+          <t>۱۴ روز و  ۷ ساعت</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615448&amp;domainType=1431&amp;needId=3400478</t>
         </is>
       </c>
     </row>
@@ -1472,12 +1472,12 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>۳ روز و  ۸ ساعت</t>
+          <t>۳ روز و  ۷ ساعت</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615437&amp;domainType=1431&amp;needId=3400470</t>
         </is>
       </c>
     </row>
@@ -1530,12 +1530,12 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>۴ روز و  ۱۵ ساعت</t>
+          <t>۴ روز و  ۱۴ ساعت</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615428&amp;domainType=1431&amp;needId=3400462</t>
         </is>
       </c>
     </row>
@@ -1588,12 +1588,12 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>۱۰ روز و  ۱۷ ساعت</t>
+          <t>۱۰ روز و  ۱۶ ساعت</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615345&amp;domainType=1431&amp;needId=3400395</t>
         </is>
       </c>
     </row>
@@ -1646,12 +1646,12 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>۱۶ روز و  ۸ ساعت</t>
+          <t>۱۶ روز و  ۷ ساعت</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615420&amp;domainType=1431&amp;needId=3400458</t>
         </is>
       </c>
     </row>
@@ -1704,12 +1704,12 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>۷ روز و  ۱۰ ساعت</t>
+          <t>۷ روز و  ۹ ساعت</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615402&amp;domainType=1431&amp;needId=3400445</t>
         </is>
       </c>
     </row>
@@ -1762,12 +1762,12 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>۱ روز و  ۱۸ ساعت</t>
+          <t>۱ روز و  ۱۷ ساعت</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615374&amp;domainType=1431&amp;needId=3400423</t>
         </is>
       </c>
     </row>
@@ -1820,12 +1820,12 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>۴ روز و  ۱۵ ساعت</t>
+          <t>۴ روز و  ۱۴ ساعت</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615396&amp;domainType=1431&amp;needId=3400440</t>
         </is>
       </c>
     </row>
@@ -1878,12 +1878,12 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>۲ روز و  ۱۰ ساعت</t>
+          <t>۲ روز و  ۹ ساعت</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615358&amp;domainType=1431&amp;needId=3400408</t>
         </is>
       </c>
     </row>
@@ -1936,12 +1936,12 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>۲ روز و  ۱۹ ساعت</t>
+          <t>۲ روز و  ۱۸ ساعت</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4613380&amp;domainType=1431&amp;needId=3398966</t>
         </is>
       </c>
     </row>
@@ -1994,12 +1994,12 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>۷ روز و  ۱۰ ساعت</t>
+          <t>۷ روز و  ۹ ساعت</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615366&amp;domainType=1431&amp;needId=3400415</t>
         </is>
       </c>
     </row>
@@ -2052,12 +2052,12 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>۱۷ روز و  ۸ ساعت</t>
+          <t>۱۷ روز و  ۷ ساعت</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615352&amp;domainType=1431&amp;needId=3400402</t>
         </is>
       </c>
     </row>
@@ -2110,12 +2110,12 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>۲ روز و  ۸ ساعت</t>
+          <t>۲ روز و  ۷ ساعت</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615267&amp;domainType=1431&amp;needId=3400330</t>
         </is>
       </c>
     </row>
@@ -2168,12 +2168,12 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>۳ روز و  ۱۰ ساعت</t>
+          <t>۳ روز و  ۹ ساعت</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4560401&amp;domainType=1431&amp;needId=3360837</t>
         </is>
       </c>
     </row>
@@ -2226,12 +2226,12 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>۶ روز و  ۱۵ ساعت</t>
+          <t>۶ روز و  ۱۴ ساعت</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615309&amp;domainType=1431&amp;needId=3400371</t>
         </is>
       </c>
     </row>
@@ -2284,12 +2284,12 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>۲ روز و  ۱۳ ساعت</t>
+          <t>۲ روز و  ۱۲ ساعت</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615182&amp;domainType=1431&amp;needId=3400285</t>
         </is>
       </c>
     </row>
@@ -2342,12 +2342,12 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>۲ روز و  ۱۵ ساعت</t>
+          <t>۲ روز و  ۱۴ ساعت</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615293&amp;domainType=1431&amp;needId=3400370</t>
         </is>
       </c>
     </row>
@@ -2400,12 +2400,12 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>۳ روز و  ۱۵ ساعت</t>
+          <t>۳ روز و  ۱۴ ساعت</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615245&amp;domainType=1431&amp;needId=3400317</t>
         </is>
       </c>
     </row>
@@ -2458,12 +2458,12 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>۲ روز و  ۱۰ ساعت</t>
+          <t>۲ روز و  ۹ ساعت</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615253&amp;domainType=1431&amp;needId=3400320</t>
         </is>
       </c>
     </row>
@@ -2516,12 +2516,12 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>۶ روز و  ۹ ساعت</t>
+          <t>۶ روز و  ۸ ساعت</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615151&amp;domainType=1431&amp;needId=3400241</t>
         </is>
       </c>
     </row>
@@ -2574,12 +2574,12 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>۶ روز و  ۱۱ ساعت</t>
+          <t>۶ روز و  ۱۰ ساعت</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615088&amp;domainType=1431&amp;needId=3400189</t>
         </is>
       </c>
     </row>
@@ -2632,12 +2632,12 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>۷ روز و  ۱۱ ساعت</t>
+          <t>۷ روز و  ۱۰ ساعت</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615231&amp;domainType=1431&amp;needId=3400305</t>
         </is>
       </c>
     </row>
@@ -2690,12 +2690,12 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>۳ روز و  ۱۵ ساعت</t>
+          <t>۳ روز و  ۱۴ ساعت</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4614810&amp;domainType=1431&amp;needId=3399965</t>
         </is>
       </c>
     </row>
@@ -2748,12 +2748,12 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>۳ روز و  ۱۵ ساعت</t>
+          <t>۳ روز و  ۱۴ ساعت</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4614661&amp;domainType=1431&amp;needId=3399861</t>
         </is>
       </c>
     </row>
@@ -2806,12 +2806,12 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>۲ روز و  ۹ ساعت</t>
+          <t>۲ روز و  ۸ ساعت</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615228&amp;domainType=1431&amp;needId=3400308</t>
         </is>
       </c>
     </row>
@@ -2864,12 +2864,12 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>۴ روز و  ۱۱ ساعت</t>
+          <t>۴ روز و  ۱۰ ساعت</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615234&amp;domainType=1431&amp;needId=3400307</t>
         </is>
       </c>
     </row>
@@ -2922,12 +2922,12 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>۶ روز و  ۱۸ ساعت</t>
+          <t>۶ روز و  ۱۷ ساعت</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4611437&amp;domainType=1431&amp;needId=3397514</t>
         </is>
       </c>
     </row>
@@ -2980,12 +2980,12 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>۱ روز و  ۱۷ ساعت</t>
+          <t>۱ روز و  ۱۶ ساعت</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615223&amp;domainType=1431&amp;needId=3400299</t>
         </is>
       </c>
     </row>
@@ -3038,12 +3038,12 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>۶ روز و  ۱۳ ساعت</t>
+          <t>۶ روز و  ۱۲ ساعت</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615222&amp;domainType=1431&amp;needId=3400298</t>
         </is>
       </c>
     </row>
@@ -3096,12 +3096,12 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>۱ روز و  ۱۷ ساعت</t>
+          <t>۱ روز و  ۱۵ ساعت</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615214&amp;domainType=1431&amp;needId=3400293</t>
         </is>
       </c>
     </row>
@@ -3154,12 +3154,12 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>۲ روز و  ۹ ساعت</t>
+          <t>۲ روز و  ۸ ساعت</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4612567&amp;domainType=1431&amp;needId=3398319</t>
         </is>
       </c>
     </row>
@@ -3212,12 +3212,12 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>۶ روز و  ۱۳ ساعت</t>
+          <t>۶ روز و  ۱۲ ساعت</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615204&amp;domainType=1431&amp;needId=3400282</t>
         </is>
       </c>
     </row>
@@ -3270,12 +3270,12 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>۴ روز و  ۱۳ ساعت</t>
+          <t>۴ روز و  ۱۲ ساعت</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615174&amp;domainType=1431&amp;needId=3400263</t>
         </is>
       </c>
     </row>
@@ -3328,12 +3328,12 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>۳ روز و  ۱۱ ساعت</t>
+          <t>۳ روز و  ۱۰ ساعت</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615159&amp;domainType=1431&amp;needId=3400249</t>
         </is>
       </c>
     </row>
@@ -3386,12 +3386,12 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>۳ روز و  ۱۰ ساعت</t>
+          <t>۳ روز و  ۹ ساعت</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615170&amp;domainType=1431&amp;needId=3400262</t>
         </is>
       </c>
     </row>
@@ -3444,12 +3444,12 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>۱ روز و  ۱۶ ساعت</t>
+          <t>۱ روز و  ۱۵ ساعت</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615168&amp;domainType=1431&amp;needId=3400258</t>
         </is>
       </c>
     </row>
@@ -3502,12 +3502,12 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>۲ روز و  ۱۰ ساعت</t>
+          <t>۲ روز و  ۹ ساعت</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615153&amp;domainType=1431&amp;needId=3400244</t>
         </is>
       </c>
     </row>
@@ -3560,12 +3560,12 @@
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>۸ روز و  ۱۳ ساعت</t>
+          <t>۸ روز و  ۱۲ ساعت</t>
         </is>
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4596566&amp;domainType=1431&amp;needId=3400206</t>
         </is>
       </c>
     </row>
@@ -3618,12 +3618,12 @@
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>۳ روز و  ۱۱ ساعت</t>
+          <t>۳ روز و  ۱۰ ساعت</t>
         </is>
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615137&amp;domainType=1431&amp;needId=3400229</t>
         </is>
       </c>
     </row>
@@ -3676,12 +3676,12 @@
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>۹ روز و  ۱۰ ساعت</t>
+          <t>۹ روز و  ۹ ساعت</t>
         </is>
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615119&amp;domainType=1431&amp;needId=3400213</t>
         </is>
       </c>
     </row>
@@ -3734,12 +3734,12 @@
       </c>
       <c r="K57" t="inlineStr">
         <is>
-          <t>۶ روز و  ۱۳ ساعت</t>
+          <t>۶ روز و  ۱۲ ساعت</t>
         </is>
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4613760&amp;domainType=1431&amp;needId=3400218</t>
         </is>
       </c>
     </row>
@@ -3792,12 +3792,12 @@
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>۳ روز و  ۱۱ ساعت</t>
+          <t>۳ روز و  ۱۰ ساعت</t>
         </is>
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615112&amp;domainType=1431&amp;needId=3400209</t>
         </is>
       </c>
     </row>
@@ -3850,12 +3850,12 @@
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>۱۰ روز و  ۱۱ ساعت</t>
+          <t>۱۰ روز و  ۱۰ ساعت</t>
         </is>
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615096&amp;domainType=1431&amp;needId=3400203</t>
         </is>
       </c>
     </row>
@@ -3908,12 +3908,12 @@
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>۳ روز و  ۸ ساعت</t>
+          <t>۳ روز و  ۷ ساعت</t>
         </is>
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615053&amp;domainType=1431&amp;needId=3400156</t>
         </is>
       </c>
     </row>
@@ -3966,12 +3966,12 @@
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>۶ روز و  ۱۳ ساعت</t>
+          <t>۶ روز و  ۱۲ ساعت</t>
         </is>
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615074&amp;domainType=1431&amp;needId=3400172</t>
         </is>
       </c>
     </row>
@@ -4024,12 +4024,12 @@
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>۳ روز</t>
+          <t>۲ روز و  ۲۳ ساعت</t>
         </is>
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615061&amp;domainType=1431&amp;needId=3400177</t>
         </is>
       </c>
     </row>
@@ -4082,12 +4082,12 @@
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>۲ روز و  ۱۰ ساعت</t>
+          <t>۲ روز و  ۹ ساعت</t>
         </is>
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615080&amp;domainType=1431&amp;needId=3400184</t>
         </is>
       </c>
     </row>
@@ -4140,12 +4140,12 @@
       </c>
       <c r="K64" t="inlineStr">
         <is>
-          <t>۳ روز و  ۱۱ ساعت</t>
+          <t>۳ روز و  ۱۰ ساعت</t>
         </is>
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4518747&amp;domainType=1431&amp;needId=3331405</t>
         </is>
       </c>
     </row>
@@ -4198,12 +4198,12 @@
       </c>
       <c r="K65" t="inlineStr">
         <is>
-          <t>۶ روز و  ۹ ساعت</t>
+          <t>۶ روز و  ۸ ساعت</t>
         </is>
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615015&amp;domainType=1431&amp;needId=3400123</t>
         </is>
       </c>
     </row>
@@ -4256,12 +4256,12 @@
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>۳ روز و  ۹ ساعت</t>
+          <t>۳ روز و  ۸ ساعت</t>
         </is>
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615040&amp;domainType=1431&amp;needId=3400151</t>
         </is>
       </c>
     </row>
@@ -4314,12 +4314,12 @@
       </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>۱ روز و  ۱۶ ساعت</t>
+          <t>۱ روز و  ۱۵ ساعت</t>
         </is>
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4614966&amp;domainType=1431&amp;needId=3400090</t>
         </is>
       </c>
     </row>
@@ -4372,12 +4372,12 @@
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>۲ روز و  ۱۰ ساعت</t>
+          <t>۲ روز و  ۹ ساعت</t>
         </is>
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615033&amp;domainType=1431&amp;needId=3400138</t>
         </is>
       </c>
     </row>
@@ -4430,12 +4430,12 @@
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>۹ روز و  ۹ ساعت</t>
+          <t>۹ روز و  ۸ ساعت</t>
         </is>
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615003&amp;domainType=1431&amp;needId=3400127</t>
         </is>
       </c>
     </row>
@@ -4488,12 +4488,12 @@
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>۲ روز و  ۹ ساعت</t>
+          <t>۲ روز و  ۸ ساعت</t>
         </is>
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4614917&amp;domainType=1431&amp;needId=3400068</t>
         </is>
       </c>
     </row>
@@ -4546,12 +4546,12 @@
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>۳ روز و  ۹ ساعت</t>
+          <t>۳ روز و  ۸ ساعت</t>
         </is>
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4615017&amp;domainType=1431&amp;needId=3400131</t>
         </is>
       </c>
     </row>
@@ -4604,12 +4604,12 @@
       </c>
       <c r="K72" t="inlineStr">
         <is>
-          <t>۳ روز و  ۱۲ ساعت</t>
+          <t>۳ روز و  ۱۱ ساعت</t>
         </is>
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4614977&amp;domainType=1431&amp;needId=3400108</t>
         </is>
       </c>
     </row>
@@ -4662,12 +4662,12 @@
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>۶ روز و  ۱۳ ساعت</t>
+          <t>۶ روز و  ۱۲ ساعت</t>
         </is>
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4614996&amp;domainType=1431&amp;needId=3400107</t>
         </is>
       </c>
     </row>
@@ -4720,12 +4720,12 @@
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>۳ روز و  ۹ ساعت</t>
+          <t>۳ روز و  ۸ ساعت</t>
         </is>
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4614991&amp;domainType=1431&amp;needId=3400112</t>
         </is>
       </c>
     </row>
@@ -4778,12 +4778,12 @@
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>۱۴ روز و  ۱۱ ساعت</t>
+          <t>۱۴ روز و  ۱۰ ساعت</t>
         </is>
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4614866&amp;domainType=1431&amp;needId=3400005</t>
         </is>
       </c>
     </row>
@@ -4836,12 +4836,12 @@
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>۴ روز و  ۹ ساعت</t>
+          <t>۴ روز و  ۸ ساعت</t>
         </is>
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4614843&amp;domainType=1431&amp;needId=3400022</t>
         </is>
       </c>
     </row>
@@ -4894,12 +4894,12 @@
       </c>
       <c r="K77" t="inlineStr">
         <is>
-          <t>۳ روز و  ۹ ساعت</t>
+          <t>۳ روز و  ۸ ساعت</t>
         </is>
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4614876&amp;domainType=1431&amp;needId=3400014</t>
         </is>
       </c>
     </row>
@@ -4952,12 +4952,12 @@
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>۲ روز و  ۱۷ ساعت</t>
+          <t>۲ روز و  ۱۶ ساعت</t>
         </is>
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4613681&amp;domainType=1431&amp;needId=3399122</t>
         </is>
       </c>
     </row>
@@ -5010,12 +5010,12 @@
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>۲ روز و  ۱۶ ساعت</t>
+          <t>۲ روز و  ۱۵ ساعت</t>
         </is>
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4614409&amp;domainType=1431&amp;needId=3399659</t>
         </is>
       </c>
     </row>
@@ -5068,12 +5068,12 @@
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>۳ روز و  ۹ ساعت</t>
+          <t>۳ روز و  ۸ ساعت</t>
         </is>
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4614876&amp;domainType=1431&amp;needId=3400014</t>
         </is>
       </c>
     </row>
@@ -5126,12 +5126,12 @@
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>۲ روز و  ۱۷ ساعت</t>
+          <t>۲ روز و  ۱۶ ساعت</t>
         </is>
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4613681&amp;domainType=1431&amp;needId=3399122</t>
         </is>
       </c>
     </row>
@@ -5184,1752 +5184,12 @@
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>۲ روز و  ۱۶ ساعت</t>
+          <t>۲ روز و  ۱۵ ساعت</t>
         </is>
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>۵۸۷</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۹۳۵۶۷۰۰۰۸۱۹</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>البسه کار &amp; #40;زمستانی&amp; #41; طبق شرح پی...</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>شرکت نفت و گاز اروندان</t>
-        </is>
-      </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>خوزستان</t>
-        </is>
-      </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H83" t="inlineStr">
-        <is>
-          <t>پوشاک و کفش</t>
-        </is>
-      </c>
-      <c r="I83" t="inlineStr"/>
-      <c r="J83" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K83" t="inlineStr">
-        <is>
-          <t>۳ روز و  ۹ ساعت</t>
-        </is>
-      </c>
-      <c r="L83" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>۵۹۱</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۹۴۳۷۶۰۰۰۰۰۲</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>36 قلم لوازم التحریر به شرح اس...</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>بازرگانی گاز ایران</t>
-        </is>
-      </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>تهران</t>
-        </is>
-      </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>تجهیزات و وسایل ت...</t>
-        </is>
-      </c>
-      <c r="I84" t="inlineStr"/>
-      <c r="J84" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K84" t="inlineStr">
-        <is>
-          <t>۲ روز و  ۱۷ ساعت</t>
-        </is>
-      </c>
-      <c r="L84" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>۵۹۶</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۰۳۶۳۶۰۰۰۰۷۰</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>خرید5 دستگاه اجاق گاز مدلSF51،...</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>مدیریت شعب بانک مسکن در استان اذربایجان شرقی</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>آذربایجان شرقی</t>
-        </is>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t>تجهیزات خانگی، اد...</t>
-        </is>
-      </c>
-      <c r="I85" t="inlineStr"/>
-      <c r="J85" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K85" t="inlineStr">
-        <is>
-          <t>۲ روز و  ۱۶ ساعت</t>
-        </is>
-      </c>
-      <c r="L85" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>۵۸۷</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۹۳۵۶۷۰۰۰۸۱۹</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>البسه کار &amp; #40;زمستانی&amp; #41; طبق شرح پی...</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>شرکت نفت و گاز اروندان</t>
-        </is>
-      </c>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>خوزستان</t>
-        </is>
-      </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H86" t="inlineStr">
-        <is>
-          <t>پوشاک و کفش</t>
-        </is>
-      </c>
-      <c r="I86" t="inlineStr"/>
-      <c r="J86" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K86" t="inlineStr">
-        <is>
-          <t>۳ روز و  ۹ ساعت</t>
-        </is>
-      </c>
-      <c r="L86" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>۵۹۱</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۹۴۳۷۶۰۰۰۰۰۲</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>36 قلم لوازم التحریر به شرح اس...</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>بازرگانی گاز ایران</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>تهران</t>
-        </is>
-      </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H87" t="inlineStr">
-        <is>
-          <t>تجهیزات و وسایل ت...</t>
-        </is>
-      </c>
-      <c r="I87" t="inlineStr"/>
-      <c r="J87" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K87" t="inlineStr">
-        <is>
-          <t>۲ روز و  ۱۷ ساعت</t>
-        </is>
-      </c>
-      <c r="L87" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>۵۹۶</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۰۳۶۳۶۰۰۰۰۷۰</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>خرید5 دستگاه اجاق گاز مدلSF51،...</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>مدیریت شعب بانک مسکن در استان اذربایجان شرقی</t>
-        </is>
-      </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>آذربایجان شرقی</t>
-        </is>
-      </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H88" t="inlineStr">
-        <is>
-          <t>تجهیزات خانگی، اد...</t>
-        </is>
-      </c>
-      <c r="I88" t="inlineStr"/>
-      <c r="J88" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K88" t="inlineStr">
-        <is>
-          <t>۲ روز و  ۱۶ ساعت</t>
-        </is>
-      </c>
-      <c r="L88" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>۵۸۷</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۹۳۵۶۷۰۰۰۸۱۹</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>البسه کار &amp; #40;زمستانی&amp; #41; طبق شرح پی...</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>شرکت نفت و گاز اروندان</t>
-        </is>
-      </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>خوزستان</t>
-        </is>
-      </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t>پوشاک و کفش</t>
-        </is>
-      </c>
-      <c r="I89" t="inlineStr"/>
-      <c r="J89" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K89" t="inlineStr">
-        <is>
-          <t>۳ روز و  ۹ ساعت</t>
-        </is>
-      </c>
-      <c r="L89" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>۵۹۱</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۹۴۳۷۶۰۰۰۰۰۲</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>36 قلم لوازم التحریر به شرح اس...</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>بازرگانی گاز ایران</t>
-        </is>
-      </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>تهران</t>
-        </is>
-      </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t>تجهیزات و وسایل ت...</t>
-        </is>
-      </c>
-      <c r="I90" t="inlineStr"/>
-      <c r="J90" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K90" t="inlineStr">
-        <is>
-          <t>۲ روز و  ۱۷ ساعت</t>
-        </is>
-      </c>
-      <c r="L90" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>۵۹۶</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۰۳۶۳۶۰۰۰۰۷۰</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>خرید5 دستگاه اجاق گاز مدلSF51،...</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>مدیریت شعب بانک مسکن در استان اذربایجان شرقی</t>
-        </is>
-      </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>آذربایجان شرقی</t>
-        </is>
-      </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H91" t="inlineStr">
-        <is>
-          <t>تجهیزات خانگی، اد...</t>
-        </is>
-      </c>
-      <c r="I91" t="inlineStr"/>
-      <c r="J91" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K91" t="inlineStr">
-        <is>
-          <t>۲ روز و  ۱۶ ساعت</t>
-        </is>
-      </c>
-      <c r="L91" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>۵۸۷</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۹۳۵۶۷۰۰۰۸۱۹</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>البسه کار &amp; #40;زمستانی&amp; #41; طبق شرح پی...</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>شرکت نفت و گاز اروندان</t>
-        </is>
-      </c>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>خوزستان</t>
-        </is>
-      </c>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H92" t="inlineStr">
-        <is>
-          <t>پوشاک و کفش</t>
-        </is>
-      </c>
-      <c r="I92" t="inlineStr"/>
-      <c r="J92" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K92" t="inlineStr">
-        <is>
-          <t>۳ روز و  ۹ ساعت</t>
-        </is>
-      </c>
-      <c r="L92" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>۵۹۱</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۹۴۳۷۶۰۰۰۰۰۲</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>36 قلم لوازم التحریر به شرح اس...</t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>بازرگانی گاز ایران</t>
-        </is>
-      </c>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>تهران</t>
-        </is>
-      </c>
-      <c r="F93" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H93" t="inlineStr">
-        <is>
-          <t>تجهیزات و وسایل ت...</t>
-        </is>
-      </c>
-      <c r="I93" t="inlineStr"/>
-      <c r="J93" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K93" t="inlineStr">
-        <is>
-          <t>۲ روز و  ۱۷ ساعت</t>
-        </is>
-      </c>
-      <c r="L93" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>۵۹۶</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۰۳۶۳۶۰۰۰۰۷۰</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>خرید5 دستگاه اجاق گاز مدلSF51،...</t>
-        </is>
-      </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>مدیریت شعب بانک مسکن در استان اذربایجان شرقی</t>
-        </is>
-      </c>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>آذربایجان شرقی</t>
-        </is>
-      </c>
-      <c r="F94" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H94" t="inlineStr">
-        <is>
-          <t>تجهیزات خانگی، اد...</t>
-        </is>
-      </c>
-      <c r="I94" t="inlineStr"/>
-      <c r="J94" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K94" t="inlineStr">
-        <is>
-          <t>۲ روز و  ۱۶ ساعت</t>
-        </is>
-      </c>
-      <c r="L94" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>۵۸۷</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۹۳۵۶۷۰۰۰۸۱۹</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>البسه کار &amp; #40;زمستانی&amp; #41; طبق شرح پی...</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>شرکت نفت و گاز اروندان</t>
-        </is>
-      </c>
-      <c r="E95" t="inlineStr">
-        <is>
-          <t>خوزستان</t>
-        </is>
-      </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H95" t="inlineStr">
-        <is>
-          <t>پوشاک و کفش</t>
-        </is>
-      </c>
-      <c r="I95" t="inlineStr"/>
-      <c r="J95" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K95" t="inlineStr">
-        <is>
-          <t>۳ روز و  ۹ ساعت</t>
-        </is>
-      </c>
-      <c r="L95" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>۵۹۱</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۹۴۳۷۶۰۰۰۰۰۲</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>36 قلم لوازم التحریر به شرح اس...</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>بازرگانی گاز ایران</t>
-        </is>
-      </c>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>تهران</t>
-        </is>
-      </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H96" t="inlineStr">
-        <is>
-          <t>تجهیزات و وسایل ت...</t>
-        </is>
-      </c>
-      <c r="I96" t="inlineStr"/>
-      <c r="J96" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K96" t="inlineStr">
-        <is>
-          <t>۲ روز و  ۱۷ ساعت</t>
-        </is>
-      </c>
-      <c r="L96" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>۵۹۶</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۰۳۶۳۶۰۰۰۰۷۰</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>خرید5 دستگاه اجاق گاز مدلSF51،...</t>
-        </is>
-      </c>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>مدیریت شعب بانک مسکن در استان اذربایجان شرقی</t>
-        </is>
-      </c>
-      <c r="E97" t="inlineStr">
-        <is>
-          <t>آذربایجان شرقی</t>
-        </is>
-      </c>
-      <c r="F97" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H97" t="inlineStr">
-        <is>
-          <t>تجهیزات خانگی، اد...</t>
-        </is>
-      </c>
-      <c r="I97" t="inlineStr"/>
-      <c r="J97" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K97" t="inlineStr">
-        <is>
-          <t>۲ روز و  ۱۶ ساعت</t>
-        </is>
-      </c>
-      <c r="L97" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>۵۸۷</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۹۳۵۶۷۰۰۰۸۱۹</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>البسه کار &amp; #40;زمستانی&amp; #41; طبق شرح پی...</t>
-        </is>
-      </c>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>شرکت نفت و گاز اروندان</t>
-        </is>
-      </c>
-      <c r="E98" t="inlineStr">
-        <is>
-          <t>خوزستان</t>
-        </is>
-      </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H98" t="inlineStr">
-        <is>
-          <t>پوشاک و کفش</t>
-        </is>
-      </c>
-      <c r="I98" t="inlineStr"/>
-      <c r="J98" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K98" t="inlineStr">
-        <is>
-          <t>۳ روز و  ۹ ساعت</t>
-        </is>
-      </c>
-      <c r="L98" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>۵۹۱</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۹۴۳۷۶۰۰۰۰۰۲</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>36 قلم لوازم التحریر به شرح اس...</t>
-        </is>
-      </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>بازرگانی گاز ایران</t>
-        </is>
-      </c>
-      <c r="E99" t="inlineStr">
-        <is>
-          <t>تهران</t>
-        </is>
-      </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H99" t="inlineStr">
-        <is>
-          <t>تجهیزات و وسایل ت...</t>
-        </is>
-      </c>
-      <c r="I99" t="inlineStr"/>
-      <c r="J99" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K99" t="inlineStr">
-        <is>
-          <t>۲ روز و  ۱۷ ساعت</t>
-        </is>
-      </c>
-      <c r="L99" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>۵۹۶</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۰۳۶۳۶۰۰۰۰۷۰</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>خرید5 دستگاه اجاق گاز مدلSF51،...</t>
-        </is>
-      </c>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>مدیریت شعب بانک مسکن در استان اذربایجان شرقی</t>
-        </is>
-      </c>
-      <c r="E100" t="inlineStr">
-        <is>
-          <t>آذربایجان شرقی</t>
-        </is>
-      </c>
-      <c r="F100" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H100" t="inlineStr">
-        <is>
-          <t>تجهیزات خانگی، اد...</t>
-        </is>
-      </c>
-      <c r="I100" t="inlineStr"/>
-      <c r="J100" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K100" t="inlineStr">
-        <is>
-          <t>۲ روز و  ۱۶ ساعت</t>
-        </is>
-      </c>
-      <c r="L100" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>۵۸۷</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۹۳۵۶۷۰۰۰۸۱۹</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>البسه کار &amp; #40;زمستانی&amp; #41; طبق شرح پی...</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>شرکت نفت و گاز اروندان</t>
-        </is>
-      </c>
-      <c r="E101" t="inlineStr">
-        <is>
-          <t>خوزستان</t>
-        </is>
-      </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H101" t="inlineStr">
-        <is>
-          <t>پوشاک و کفش</t>
-        </is>
-      </c>
-      <c r="I101" t="inlineStr"/>
-      <c r="J101" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K101" t="inlineStr">
-        <is>
-          <t>۳ روز و  ۹ ساعت</t>
-        </is>
-      </c>
-      <c r="L101" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>۵۹۱</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۹۴۳۷۶۰۰۰۰۰۲</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>36 قلم لوازم التحریر به شرح اس...</t>
-        </is>
-      </c>
-      <c r="D102" t="inlineStr">
-        <is>
-          <t>بازرگانی گاز ایران</t>
-        </is>
-      </c>
-      <c r="E102" t="inlineStr">
-        <is>
-          <t>تهران</t>
-        </is>
-      </c>
-      <c r="F102" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G102" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H102" t="inlineStr">
-        <is>
-          <t>تجهیزات و وسایل ت...</t>
-        </is>
-      </c>
-      <c r="I102" t="inlineStr"/>
-      <c r="J102" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K102" t="inlineStr">
-        <is>
-          <t>۲ روز و  ۱۷ ساعت</t>
-        </is>
-      </c>
-      <c r="L102" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>۵۹۶</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۰۳۶۳۶۰۰۰۰۷۰</t>
-        </is>
-      </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>خرید5 دستگاه اجاق گاز مدلSF51،...</t>
-        </is>
-      </c>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>مدیریت شعب بانک مسکن در استان اذربایجان شرقی</t>
-        </is>
-      </c>
-      <c r="E103" t="inlineStr">
-        <is>
-          <t>آذربایجان شرقی</t>
-        </is>
-      </c>
-      <c r="F103" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G103" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H103" t="inlineStr">
-        <is>
-          <t>تجهیزات خانگی، اد...</t>
-        </is>
-      </c>
-      <c r="I103" t="inlineStr"/>
-      <c r="J103" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K103" t="inlineStr">
-        <is>
-          <t>۲ روز و  ۱۶ ساعت</t>
-        </is>
-      </c>
-      <c r="L103" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>۵۸۷</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۹۳۵۶۷۰۰۰۸۱۹</t>
-        </is>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>البسه کار &amp; #40;زمستانی&amp; #41; طبق شرح پی...</t>
-        </is>
-      </c>
-      <c r="D104" t="inlineStr">
-        <is>
-          <t>شرکت نفت و گاز اروندان</t>
-        </is>
-      </c>
-      <c r="E104" t="inlineStr">
-        <is>
-          <t>خوزستان</t>
-        </is>
-      </c>
-      <c r="F104" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H104" t="inlineStr">
-        <is>
-          <t>پوشاک و کفش</t>
-        </is>
-      </c>
-      <c r="I104" t="inlineStr"/>
-      <c r="J104" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K104" t="inlineStr">
-        <is>
-          <t>۳ روز و  ۹ ساعت</t>
-        </is>
-      </c>
-      <c r="L104" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>۵۹۱</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۹۴۳۷۶۰۰۰۰۰۲</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>36 قلم لوازم التحریر به شرح اس...</t>
-        </is>
-      </c>
-      <c r="D105" t="inlineStr">
-        <is>
-          <t>بازرگانی گاز ایران</t>
-        </is>
-      </c>
-      <c r="E105" t="inlineStr">
-        <is>
-          <t>تهران</t>
-        </is>
-      </c>
-      <c r="F105" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H105" t="inlineStr">
-        <is>
-          <t>تجهیزات و وسایل ت...</t>
-        </is>
-      </c>
-      <c r="I105" t="inlineStr"/>
-      <c r="J105" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K105" t="inlineStr">
-        <is>
-          <t>۲ روز و  ۱۷ ساعت</t>
-        </is>
-      </c>
-      <c r="L105" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>۵۹۶</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۰۳۶۳۶۰۰۰۰۷۰</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>خرید5 دستگاه اجاق گاز مدلSF51،...</t>
-        </is>
-      </c>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t>مدیریت شعب بانک مسکن در استان اذربایجان شرقی</t>
-        </is>
-      </c>
-      <c r="E106" t="inlineStr">
-        <is>
-          <t>آذربایجان شرقی</t>
-        </is>
-      </c>
-      <c r="F106" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G106" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H106" t="inlineStr">
-        <is>
-          <t>تجهیزات خانگی، اد...</t>
-        </is>
-      </c>
-      <c r="I106" t="inlineStr"/>
-      <c r="J106" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K106" t="inlineStr">
-        <is>
-          <t>۲ روز و  ۱۶ ساعت</t>
-        </is>
-      </c>
-      <c r="L106" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>۵۸۷</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۹۳۵۶۷۰۰۰۸۱۹</t>
-        </is>
-      </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>البسه کار &amp; #40;زمستانی&amp; #41; طبق شرح پی...</t>
-        </is>
-      </c>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t>شرکت نفت و گاز اروندان</t>
-        </is>
-      </c>
-      <c r="E107" t="inlineStr">
-        <is>
-          <t>خوزستان</t>
-        </is>
-      </c>
-      <c r="F107" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H107" t="inlineStr">
-        <is>
-          <t>پوشاک و کفش</t>
-        </is>
-      </c>
-      <c r="I107" t="inlineStr"/>
-      <c r="J107" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K107" t="inlineStr">
-        <is>
-          <t>۳ روز و  ۹ ساعت</t>
-        </is>
-      </c>
-      <c r="L107" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>۵۹۱</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۹۴۳۷۶۰۰۰۰۰۲</t>
-        </is>
-      </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>36 قلم لوازم التحریر به شرح اس...</t>
-        </is>
-      </c>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>بازرگانی گاز ایران</t>
-        </is>
-      </c>
-      <c r="E108" t="inlineStr">
-        <is>
-          <t>تهران</t>
-        </is>
-      </c>
-      <c r="F108" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G108" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H108" t="inlineStr">
-        <is>
-          <t>تجهیزات و وسایل ت...</t>
-        </is>
-      </c>
-      <c r="I108" t="inlineStr"/>
-      <c r="J108" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K108" t="inlineStr">
-        <is>
-          <t>۲ روز و  ۱۷ ساعت</t>
-        </is>
-      </c>
-      <c r="L108" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>۵۹۶</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۰۳۶۳۶۰۰۰۰۷۰</t>
-        </is>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>خرید5 دستگاه اجاق گاز مدلSF51،...</t>
-        </is>
-      </c>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>مدیریت شعب بانک مسکن در استان اذربایجان شرقی</t>
-        </is>
-      </c>
-      <c r="E109" t="inlineStr">
-        <is>
-          <t>آذربایجان شرقی</t>
-        </is>
-      </c>
-      <c r="F109" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G109" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H109" t="inlineStr">
-        <is>
-          <t>تجهیزات خانگی، اد...</t>
-        </is>
-      </c>
-      <c r="I109" t="inlineStr"/>
-      <c r="J109" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K109" t="inlineStr">
-        <is>
-          <t>۲ روز و  ۱۶ ساعت</t>
-        </is>
-      </c>
-      <c r="L109" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>۵۸۷</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۹۳۵۶۷۰۰۰۸۱۹</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>البسه کار &amp; #40;زمستانی&amp; #41; طبق شرح پی...</t>
-        </is>
-      </c>
-      <c r="D110" t="inlineStr">
-        <is>
-          <t>شرکت نفت و گاز اروندان</t>
-        </is>
-      </c>
-      <c r="E110" t="inlineStr">
-        <is>
-          <t>خوزستان</t>
-        </is>
-      </c>
-      <c r="F110" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G110" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H110" t="inlineStr">
-        <is>
-          <t>پوشاک و کفش</t>
-        </is>
-      </c>
-      <c r="I110" t="inlineStr"/>
-      <c r="J110" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K110" t="inlineStr">
-        <is>
-          <t>۳ روز و  ۹ ساعت</t>
-        </is>
-      </c>
-      <c r="L110" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>۵۹۱</t>
-        </is>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۹۴۳۷۶۰۰۰۰۰۲</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>36 قلم لوازم التحریر به شرح اس...</t>
-        </is>
-      </c>
-      <c r="D111" t="inlineStr">
-        <is>
-          <t>بازرگانی گاز ایران</t>
-        </is>
-      </c>
-      <c r="E111" t="inlineStr">
-        <is>
-          <t>تهران</t>
-        </is>
-      </c>
-      <c r="F111" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G111" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H111" t="inlineStr">
-        <is>
-          <t>تجهیزات و وسایل ت...</t>
-        </is>
-      </c>
-      <c r="I111" t="inlineStr"/>
-      <c r="J111" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K111" t="inlineStr">
-        <is>
-          <t>۲ روز و  ۱۷ ساعت</t>
-        </is>
-      </c>
-      <c r="L111" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>۵۹۶</t>
-        </is>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>۱۱۰۲۰۰۳۶۳۶۰۰۰۰۷۰</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>خرید5 دستگاه اجاق گاز مدلSF51،...</t>
-        </is>
-      </c>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>مدیریت شعب بانک مسکن در استان اذربایجان شرقی</t>
-        </is>
-      </c>
-      <c r="E112" t="inlineStr">
-        <is>
-          <t>آذربایجان شرقی</t>
-        </is>
-      </c>
-      <c r="F112" t="inlineStr">
-        <is>
-          <t>انتخاب تامین کننده</t>
-        </is>
-      </c>
-      <c r="G112" t="inlineStr">
-        <is>
-          <t>کالا</t>
-        </is>
-      </c>
-      <c r="H112" t="inlineStr">
-        <is>
-          <t>تجهیزات خانگی، اد...</t>
-        </is>
-      </c>
-      <c r="I112" t="inlineStr"/>
-      <c r="J112" t="inlineStr">
-        <is>
-          <t>۱۴۰۲/۱۰/۲۳</t>
-        </is>
-      </c>
-      <c r="K112" t="inlineStr">
-        <is>
-          <t>۲ روز و  ۱۶ ساعت</t>
-        </is>
-      </c>
-      <c r="L112" t="inlineStr">
-        <is>
-          <t>javascript:void(0)</t>
+          <t>https://eproc.setadiran.ir/eproc/needDetailsInfoModal-load.do?reqId=4614409&amp;domainType=1431&amp;needId=3399659</t>
         </is>
       </c>
     </row>

</xml_diff>